<commit_message>
Début de la création de l'interface
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -153,12 +153,21 @@
   </si>
   <si>
     <t>Les actions modifient les statistiques du joueur + création des classes de base.</t>
+  </si>
+  <si>
+    <t>Création des classes de base tel que représenté dans le schéma de classes.</t>
+  </si>
+  <si>
+    <t>Création de petits logos pour représenter les statistiques du joueur</t>
+  </si>
+  <si>
+    <t>Début de l'interface principale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -333,6 +342,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -347,9 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -388,7 +397,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -456,7 +465,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -522,7 +531,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -596,7 +605,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -664,7 +673,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -730,7 +739,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -804,7 +813,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -872,7 +881,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -938,7 +947,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1012,7 +1021,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1080,7 +1089,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1146,7 +1155,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1220,7 +1229,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1288,7 +1297,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1354,7 +1363,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1484,23 +1493,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1536,23 +1528,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1731,49 +1706,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1784,7 +1759,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1795,18 +1770,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>2</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="18" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="3">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1817,7 +1792,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1828,7 +1803,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1839,29 +1814,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="20"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1883,7 +1858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1894,7 +1869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1905,7 +1880,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -1916,7 +1891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -1927,7 +1902,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -1938,31 +1913,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="20"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -1983,23 +1958,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2007,7 +1982,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2015,7 +1990,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2023,13 +1998,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2040,166 +2015,184 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>42765</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>42765</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>42765</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="21"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="21"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="22"/>
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="22"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2220,19 +2213,19 @@
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2240,7 +2233,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2248,7 +2241,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2256,13 +2249,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2273,168 +2266,168 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="21"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="21"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="22"/>
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="22"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2455,19 +2448,19 @@
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2475,7 +2468,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2483,7 +2476,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2491,13 +2484,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2508,166 +2501,166 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="21"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="21"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="22"/>
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="22"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2688,19 +2681,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2708,7 +2701,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2716,7 +2709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2724,13 +2717,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2741,166 +2734,166 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="20"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="21"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="21"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="21"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="22"/>
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="22"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="22"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="22"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Création de sous-menus d'action et possibilité d'acheter de la nourriture.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -158,10 +158,13 @@
     <t>Création des classes de base tel que représenté dans le schéma de classes.</t>
   </si>
   <si>
-    <t>Création de petits logos pour représenter les statistiques du joueur</t>
-  </si>
-  <si>
-    <t>Début de l'interface principale</t>
+    <t>Création de petits logos pour représenter les statistiques du joueur.</t>
+  </si>
+  <si>
+    <t>Début de l'interface principale.</t>
+  </si>
+  <si>
+    <t>Création d'un sous-menu et l'achat de nourritures affecte les statistiques.</t>
   </si>
 </sst>
 </file>
@@ -397,7 +400,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -465,7 +468,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -531,7 +534,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -605,7 +608,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -673,7 +676,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -739,7 +742,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -813,7 +816,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -881,7 +884,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -947,7 +950,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1021,7 +1024,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1089,7 +1092,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1155,7 +1158,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1229,7 +1232,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1297,7 +1300,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1363,7 +1366,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1959,7 +1962,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2049,9 +2052,15 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="12">
+        <v>42766</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -2155,7 +2164,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Mise en place d'un OnItemClick listener sur la ListView permettant d'appuyer sur les items et d'un OnTouch listener qui désactive le scroll du parent.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -165,12 +165,18 @@
   </si>
   <si>
     <t>Création d'un sous-menu et l'achat de nourritures affecte les statistiques.</t>
+  </si>
+  <si>
+    <t>Le sous-menu est désormais une listview avec un adapter.</t>
+  </si>
+  <si>
+    <t>Click listener et touch listener sur la listview pour activer le scroll et appuyer sur les items.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -308,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -348,6 +354,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -362,6 +371,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,7 +415,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -468,7 +483,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -534,7 +549,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -608,7 +623,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -676,7 +691,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -742,7 +757,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -816,7 +831,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -884,7 +899,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -950,7 +965,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1024,7 +1039,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1092,7 +1107,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1158,7 +1173,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1232,7 +1247,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1300,7 +1315,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1381,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1496,6 +1511,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1531,6 +1563,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1713,45 +1762,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1762,7 +1811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1773,7 +1822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1784,7 +1833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1795,7 +1844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1806,7 +1855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1817,29 +1866,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1850,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1861,7 +1910,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1872,7 +1921,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1883,7 +1932,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -1894,7 +1943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -1905,7 +1954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -1916,31 +1965,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="19" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="20"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -1959,25 +2008,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:C47"/>
+  <dimension ref="A6:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1985,7 +2034,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1993,7 +2042,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2001,13 +2050,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2018,7 +2067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2029,7 +2078,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2040,7 +2089,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2051,7 +2100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2062,151 +2111,158 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>42766</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
+        <v>42771</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="16">
-        <f>SUM(C14:C36)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="B36" s="21"/>
+      <c r="C36" s="16">
+        <f>SUM(C14:C35)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="17"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B41" s="22"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="23"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="23"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="23"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="B41:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2218,23 +2274,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2242,7 +2298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2250,7 +2306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2258,13 +2314,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2275,168 +2331,168 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B42" s="22"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="23"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="23"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="23"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2453,23 +2509,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2477,7 +2533,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2485,7 +2541,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2493,13 +2549,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2510,166 +2566,166 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B42" s="22"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="23"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="23"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="23"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2690,19 +2746,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2710,7 +2766,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2718,7 +2774,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2726,13 +2782,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2743,166 +2799,166 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="21"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="22"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="22"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="22"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="22"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="23"/>
+      <c r="B42" s="22"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="23"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="23"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="23"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Layout de sélection d'heure + travailler + dormir
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -171,12 +171,18 @@
   </si>
   <si>
     <t>Click listener et touch listener sur la listview pour activer le scroll et appuyer sur les items.</t>
+  </si>
+  <si>
+    <t>Création d'un layout pour chosir le nombre d'heure.</t>
+  </si>
+  <si>
+    <t>Peut travailler et dormir.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,6 +363,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -371,12 +383,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,7 +421,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -483,7 +489,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -549,7 +555,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -623,7 +629,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -691,7 +697,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -757,7 +763,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -831,7 +837,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -899,7 +905,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -965,7 +971,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1039,7 +1045,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1107,7 +1113,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1173,7 +1179,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1247,7 +1253,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1315,7 +1321,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1381,7 +1387,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1511,23 +1517,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1563,23 +1552,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1762,45 +1734,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1811,7 +1783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1822,7 +1794,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1833,7 +1805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1844,7 +1816,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1855,7 +1827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1866,29 +1838,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="21"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1899,7 +1871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1910,7 +1882,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1921,7 +1893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1932,7 +1904,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -1943,7 +1915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -1954,7 +1926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -1965,31 +1937,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="21"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -2010,23 +1982,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2034,7 +2006,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2042,7 +2014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2050,13 +2022,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2067,7 +2039,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2078,7 +2050,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2089,7 +2061,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2100,7 +2072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2111,7 +2083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2122,142 +2094,154 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="20">
         <v>42771</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="21">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="12">
+        <v>42772</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
+        <v>42773</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="19"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="21"/>
+      <c r="B36" s="23"/>
       <c r="C36" s="16">
         <f>SUM(C14:C35)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="22"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="23"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="23"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="23"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="24"/>
+      <c r="B41" s="24"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="25"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="25"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="25"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2278,19 +2262,19 @@
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2298,7 +2282,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2306,7 +2290,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2314,13 +2298,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2331,168 +2315,168 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="21"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="22"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="23"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="23"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="23"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="24"/>
+      <c r="B42" s="24"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="25"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="25"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="25"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2513,19 +2497,19 @@
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2533,7 +2517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2541,7 +2525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2549,13 +2533,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2566,166 +2550,166 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="21"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="22"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="23"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="23"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="23"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="24"/>
+      <c r="B42" s="24"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="25"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="25"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="25"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2746,19 +2730,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2766,7 +2750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2774,7 +2758,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2782,13 +2766,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2799,166 +2783,166 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="21"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="22"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="23"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="23"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="23"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="23"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="24"/>
+      <c r="B42" s="24"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="25"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="25"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="25"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="25"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Limite de statistique + Apk
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -180,12 +180,15 @@
   </si>
   <si>
     <t>Affichage du temps et modification de celui-ci.</t>
+  </si>
+  <si>
+    <t>J'ai passé beaucoup de temps sur l'interface. Je ne considère pas avoir travaillé sur le projet 21h, car j'ai perdu mon temps lors d'un cours.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -323,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,6 +390,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,7 +436,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -492,7 +504,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -558,7 +570,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -632,7 +644,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -700,7 +712,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -766,7 +778,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -840,7 +852,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -908,7 +920,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -974,7 +986,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1048,7 +1060,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1116,7 +1128,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1182,7 +1194,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1256,7 +1268,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1324,7 +1336,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1390,7 +1402,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1520,6 +1532,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1555,6 +1584,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1737,45 +1783,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1786,7 +1832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1797,7 +1843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1808,7 +1854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1819,7 +1865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1830,7 +1876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1841,7 +1887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>9</v>
       </c>
@@ -1851,19 +1897,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1874,7 +1920,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1885,7 +1931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1896,7 +1942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1907,7 +1953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -1918,7 +1964,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -1929,7 +1975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -1940,21 +1986,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
         <v>9</v>
       </c>
@@ -1964,7 +2010,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -1985,23 +2031,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2009,7 +2055,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2017,7 +2063,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2025,13 +2071,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2042,7 +2088,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2053,7 +2099,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2064,7 +2110,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2075,7 +2121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2086,7 +2132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2097,7 +2143,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>42771</v>
       </c>
@@ -2108,7 +2154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>42772</v>
       </c>
@@ -2119,7 +2165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>42773</v>
       </c>
@@ -2130,7 +2176,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>42779</v>
       </c>
@@ -2141,74 +2187,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="12">
-        <v>42780</v>
-      </c>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>9</v>
       </c>
@@ -2218,41 +2262,45 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="4"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B39" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="24"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="25"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="25"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="25"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="25"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
+      <c r="B41" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="28"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="28"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="28"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="28"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2273,19 +2321,19 @@
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2293,7 +2341,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2301,7 +2349,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2309,13 +2357,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2326,124 +2374,124 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>9</v>
       </c>
@@ -2453,40 +2501,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B42" s="24"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="25"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="25"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="25"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="25"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="26"/>
     </row>
   </sheetData>
@@ -2508,19 +2556,19 @@
       <selection activeCell="A39" sqref="A39:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2528,7 +2576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2536,7 +2584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2544,13 +2592,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2561,122 +2609,122 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>9</v>
       </c>
@@ -2686,40 +2734,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B42" s="24"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="25"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="25"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="25"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="25"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="26"/>
     </row>
   </sheetData>
@@ -2741,19 +2789,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2761,7 +2809,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2769,7 +2817,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2777,13 +2825,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2794,122 +2842,122 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>9</v>
       </c>
@@ -2919,40 +2967,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B42" s="24"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="25"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="25"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="25"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="25"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="26"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cours + Progress bars
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>J'ai passé beaucoup de temps sur l'interface. Je ne considère pas avoir travaillé sur le projet 21h, car j'ai perdu mon temps lors d'un cours.</t>
+  </si>
+  <si>
+    <t>Création des cours (Nouveau Adapter + horaire)</t>
+  </si>
+  <si>
+    <t>Création de nouveaux styles</t>
+  </si>
+  <si>
+    <t>Progress bars</t>
   </si>
 </sst>
 </file>
@@ -326,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +391,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -390,14 +408,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2031,7 +2043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2283,24 +2295,24 @@
       <c r="A41" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="24" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
+      <c r="B42" s="25"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
+      <c r="B43" s="25"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="28"/>
+      <c r="B44" s="25"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="28"/>
+      <c r="B45" s="25"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="29"/>
+      <c r="B46" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2317,8 +2329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,130 +2387,148 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>42797</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="20">
+        <v>42797</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="20">
+        <v>42797</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="15"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="15"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="15"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="15"/>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="15"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="15"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="15"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="15"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="15"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="15"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="15"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="15"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="15"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="23"/>
-      <c r="C37" s="16">
+      <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2520,22 +2550,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="25"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="25"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="26"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2753,22 +2783,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="25"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="25"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="26"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2986,22 +3016,22 @@
       <c r="A42" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="24"/>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="25"/>
+      <c r="B43" s="28"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="25"/>
+      <c r="B44" s="28"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
+      <c r="B45" s="28"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
+      <c r="B46" s="28"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="26"/>
+      <c r="B47" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Modification de la structure du code terminée.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>Je n'ai pas assez travailler comme j'aurais du, mais je ferai plus d'heures dans les prochaines itérations.</t>
+  </si>
+  <si>
+    <t>Présentation des projets.</t>
+  </si>
+  <si>
+    <t>Modifications de la structure du code terminées.</t>
   </si>
 </sst>
 </file>
@@ -396,6 +402,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -419,9 +428,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,7 +466,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -528,7 +534,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -594,7 +600,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -668,7 +674,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -736,7 +742,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -802,7 +808,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -876,7 +882,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -944,7 +950,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1010,7 +1016,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1084,7 +1090,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1152,7 +1158,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1218,7 +1224,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1292,7 +1298,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1360,7 +1366,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1426,7 +1432,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1878,10 +1884,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="24"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>43</v>
@@ -1991,10 +1997,10 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="24"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>47</v>
@@ -2243,10 +2249,10 @@
       <c r="C35" s="15"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="23" t="s">
+      <c r="A36" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="24"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="16">
         <f>SUM(C14:C35)</f>
         <v>18</v>
@@ -2273,24 +2279,24 @@
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="26" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B42" s="26"/>
+      <c r="B42" s="27"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="26"/>
+      <c r="B43" s="27"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="26"/>
+      <c r="B44" s="27"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="26"/>
+      <c r="B45" s="27"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="27"/>
+      <c r="B46" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2307,7 +2313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
@@ -2516,10 +2522,10 @@
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
         <v>10</v>
@@ -2535,7 +2541,7 @@
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="31">
+      <c r="B40" s="23">
         <v>5</v>
       </c>
     </row>
@@ -2546,24 +2552,24 @@
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="26"/>
+      <c r="B43" s="27"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="26"/>
+      <c r="B44" s="27"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="26"/>
+      <c r="B45" s="27"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="26"/>
+      <c r="B46" s="27"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="27"/>
+      <c r="B47" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2580,8 +2586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD47"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2638,128 +2644,140 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>42814</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="12">
+        <v>42815</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
+      <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="15"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="15"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="15"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="15"/>
+      <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="15"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="15"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="15"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="15"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="15"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="15"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="15"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="15"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="15"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="16">
+      <c r="B37" s="25"/>
+      <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -2781,22 +2799,22 @@
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="28"/>
+      <c r="B42" s="29"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="29"/>
+      <c r="B43" s="30"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="29"/>
+      <c r="B44" s="30"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="29"/>
+      <c r="B45" s="30"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="29"/>
+      <c r="B46" s="30"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="30"/>
+      <c r="B47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2986,10 +3004,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="25"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -3014,22 +3032,22 @@
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="28"/>
+      <c r="B42" s="29"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B43" s="29"/>
+      <c r="B43" s="30"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" s="29"/>
+      <c r="B44" s="30"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B45" s="29"/>
+      <c r="B45" s="30"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="29"/>
+      <c r="B46" s="30"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="30"/>
+      <c r="B47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Affichage des textes des événements lors de la réussite + nouveau menuHeure
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Modifications de la structure du code terminées.</t>
+  </si>
+  <si>
+    <t>Modification du menuHeure, affichage du texte des événements lors de la réussite.</t>
   </si>
 </sst>
 </file>
@@ -350,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -429,6 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +470,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -534,7 +538,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -600,7 +604,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -674,7 +678,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -742,7 +746,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -808,7 +812,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -882,7 +886,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -950,7 +954,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1016,7 +1020,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1090,7 +1094,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1158,7 +1162,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1224,7 +1228,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1298,7 +1302,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1366,7 +1370,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1432,7 +1436,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2587,7 +2591,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B16:B17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2666,9 +2670,15 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="3"/>
+      <c r="A16" s="32">
+        <v>42821</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
@@ -2777,7 +2787,7 @@
       <c r="B37" s="25"/>
       <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Liste de devoir + Début de l'assignement de ceux-ci.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Modification du menuHeure, affichage du texte des événements lors de la réussite.</t>
+  </si>
+  <si>
+    <t>Liste de devoir + Début de l'assignement de ceux-ci.</t>
   </si>
 </sst>
 </file>
@@ -353,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -432,7 +435,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +472,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -538,7 +540,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -604,7 +606,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -678,7 +680,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -746,7 +748,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -812,7 +814,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -886,7 +888,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -954,7 +956,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1020,7 +1022,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1094,7 +1096,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1162,7 +1164,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1228,7 +1230,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1302,7 +1304,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1370,7 +1372,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1436,7 +1438,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2591,7 +2593,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2670,7 +2672,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="32">
+      <c r="A16" s="12">
         <v>42821</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2681,102 +2683,108 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="12">
+        <v>42822</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="4"/>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
@@ -2787,7 +2795,7 @@
       <c r="B37" s="25"/>
       <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
-        <v>7</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Assignement des devoirs + Importation d'une librairie de progressbar + debut du style
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>Liste de devoir + Début de l'assignement de ceux-ci.</t>
+  </si>
+  <si>
+    <t>Assignement des devoirs + Importation d'une librairie de progressbar + debut du style</t>
   </si>
 </sst>
 </file>
@@ -472,7 +475,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -540,7 +543,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -606,7 +609,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -680,7 +683,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -748,7 +751,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -814,7 +817,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -888,7 +891,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -956,7 +959,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1022,7 +1025,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1096,7 +1099,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1164,7 +1167,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1230,7 +1233,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1304,7 +1307,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1372,7 +1375,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1438,7 +1441,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2593,7 +2596,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2694,9 +2697,15 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="19"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="12">
+        <v>42797</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
@@ -2795,7 +2804,7 @@
       <c r="B37" s="25"/>
       <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
-        <v>8.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ListView pour les devoirs + layout + adapter
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -216,12 +216,15 @@
   </si>
   <si>
     <t>Assignement des devoirs + Importation d'une librairie de progressbar + debut du style</t>
+  </si>
+  <si>
+    <t>ListView pour les devoirs + layout + adapter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -475,7 +478,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -543,7 +546,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -609,7 +612,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -683,7 +686,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -751,7 +754,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -817,7 +820,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -891,7 +894,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -959,7 +962,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1025,7 +1028,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1099,7 +1102,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1167,7 +1170,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1233,7 +1236,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1307,7 +1310,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1375,7 +1378,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1441,7 +1444,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1571,6 +1574,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1606,6 +1626,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1788,45 +1825,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1837,7 +1874,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1848,7 +1885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1859,7 +1896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1870,7 +1907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1881,7 +1918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1892,7 +1929,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>9</v>
       </c>
@@ -1902,19 +1939,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1925,7 +1962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1936,7 +1973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1947,7 +1984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1958,7 +1995,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -1969,7 +2006,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -1980,7 +2017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -1991,21 +2028,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>9</v>
       </c>
@@ -2015,7 +2052,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -2040,19 +2077,19 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2060,7 +2097,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2068,7 +2105,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2076,13 +2113,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2093,7 +2130,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2104,7 +2141,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2115,7 +2152,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2126,7 +2163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2137,7 +2174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2148,7 +2185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>42771</v>
       </c>
@@ -2159,7 +2196,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>42772</v>
       </c>
@@ -2170,7 +2207,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>42773</v>
       </c>
@@ -2181,7 +2218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>42779</v>
       </c>
@@ -2192,72 +2229,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>9</v>
       </c>
@@ -2267,13 +2304,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2281,10 +2318,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2292,19 +2329,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="27"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="28"/>
     </row>
   </sheetData>
@@ -2326,19 +2363,19 @@
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2346,7 +2383,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2354,7 +2391,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2362,13 +2399,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2379,7 +2416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42797</v>
       </c>
@@ -2390,7 +2427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>42797</v>
       </c>
@@ -2401,7 +2438,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>42797</v>
       </c>
@@ -2412,7 +2449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>42798</v>
       </c>
@@ -2423,7 +2460,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>42808</v>
       </c>
@@ -2434,7 +2471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>42814</v>
       </c>
@@ -2445,92 +2482,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
@@ -2540,13 +2577,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2554,10 +2591,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
@@ -2565,19 +2602,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="27"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="28"/>
     </row>
   </sheetData>
@@ -2596,22 +2633,22 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2619,7 +2656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2627,7 +2664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2635,13 +2672,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2652,7 +2689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42814</v>
       </c>
@@ -2663,7 +2700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42815</v>
       </c>
@@ -2674,7 +2711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42821</v>
       </c>
@@ -2685,7 +2722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42822</v>
       </c>
@@ -2696,7 +2733,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>42797</v>
       </c>
@@ -2707,140 +2744,146 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="19"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>42830</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="29"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="30"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="30"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
     </row>
   </sheetData>
@@ -2862,19 +2905,19 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2882,7 +2925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2890,7 +2933,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2898,13 +2941,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2915,122 +2958,122 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="C14" s="15"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="15"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="15"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="15"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="15"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="15"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="15"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
@@ -3040,40 +3083,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="29"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="30"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="30"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Les devoirs donnent de la connaissance pour un matière en particulié.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -231,12 +231,15 @@
   </si>
   <si>
     <t>Les devoirs peuvent être complété + Penser comment terminer le jeu(Récompense des devoirs, examen, connaissance...)</t>
+  </si>
+  <si>
+    <t>Les devoirs donnent de la connaissance pour un matière en particulié.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -490,7 +493,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -558,7 +561,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -624,7 +627,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -698,7 +701,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -766,7 +769,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -832,7 +835,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -906,7 +909,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -974,7 +977,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1040,7 +1043,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1114,7 +1117,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1182,7 +1185,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1248,7 +1251,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1322,7 +1325,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1390,7 +1393,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1456,7 +1459,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1586,23 +1589,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1638,23 +1624,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1837,45 +1806,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1886,7 +1855,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1897,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1908,7 +1877,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1919,7 +1888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1930,7 +1899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1941,7 +1910,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>9</v>
       </c>
@@ -1951,19 +1920,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1974,7 +1943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1985,7 +1954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1996,7 +1965,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -2007,7 +1976,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -2018,7 +1987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -2029,7 +1998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -2040,21 +2009,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>9</v>
       </c>
@@ -2064,7 +2033,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -2089,19 +2058,19 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2109,7 +2078,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2117,7 +2086,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2125,13 +2094,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2142,7 +2111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2153,7 +2122,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2164,7 +2133,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2175,7 +2144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2186,7 +2155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2197,7 +2166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>42771</v>
       </c>
@@ -2208,7 +2177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>42772</v>
       </c>
@@ -2219,7 +2188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>42773</v>
       </c>
@@ -2230,7 +2199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>42779</v>
       </c>
@@ -2241,72 +2210,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>9</v>
       </c>
@@ -2316,13 +2285,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2330,10 +2299,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2341,19 +2310,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="27"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="27"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="27"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="27"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="28"/>
     </row>
   </sheetData>
@@ -2375,19 +2344,19 @@
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2395,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2403,7 +2372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2411,13 +2380,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2428,7 +2397,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42797</v>
       </c>
@@ -2439,7 +2408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <v>42797</v>
       </c>
@@ -2450,7 +2419,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>42797</v>
       </c>
@@ -2461,7 +2430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>42798</v>
       </c>
@@ -2472,7 +2441,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>42808</v>
       </c>
@@ -2483,7 +2452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>42814</v>
       </c>
@@ -2494,92 +2463,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="22"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
@@ -2589,13 +2558,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2603,10 +2572,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
@@ -2614,19 +2583,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="27"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="27"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="27"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="27"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="28"/>
     </row>
   </sheetData>
@@ -2644,23 +2613,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2668,7 +2637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2676,7 +2645,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2684,13 +2653,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2701,7 +2670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42814</v>
       </c>
@@ -2712,7 +2681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42815</v>
       </c>
@@ -2723,7 +2692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42821</v>
       </c>
@@ -2734,7 +2703,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42822</v>
       </c>
@@ -2745,7 +2714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42797</v>
       </c>
@@ -2756,7 +2725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>42830</v>
       </c>
@@ -2767,7 +2736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>42833</v>
       </c>
@@ -2778,7 +2747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>42834</v>
       </c>
@@ -2789,7 +2758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="20">
         <v>42834</v>
       </c>
@@ -2800,72 +2769,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="4"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>9</v>
       </c>
@@ -2875,13 +2842,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2889,10 +2856,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2900,19 +2867,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="30"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="30"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="30"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="30"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="31"/>
     </row>
   </sheetData>
@@ -2930,23 +2897,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2954,7 +2921,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2962,7 +2929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2970,13 +2937,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2987,165 +2954,171 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>42836</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="23"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="23"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="23"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="23"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="23"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="23"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="23"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="23"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="23"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="15"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="23"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="15"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="23"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
-      <c r="C27" s="15"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="23"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
-      <c r="C28" s="15"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="15"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="23"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="23"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="15"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="23"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
-      <c r="C32" s="15"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="23"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
-      <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="23"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
-      <c r="C34" s="15"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="23"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
-      <c r="C35" s="15"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="23"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="23"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="29"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="30"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="30"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="30"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="30"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="31"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des examens + Début du layout pour les faire.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>Les devoirs donnent de la connaissance pour un matière en particulié.</t>
+  </si>
+  <si>
+    <t>Ajout des examens + début du layout pour les faire.</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,6 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,7 +497,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -561,7 +565,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -627,7 +631,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -701,7 +705,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -769,7 +773,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -835,7 +839,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -909,7 +913,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -977,7 +981,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1043,7 +1047,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1117,7 +1121,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1185,7 +1189,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1251,7 +1255,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1325,7 +1329,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1393,7 +1397,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1459,7 +1463,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1802,7 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -2898,7 +2902,7 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2966,9 +2970,15 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="23"/>
+      <c r="A15" s="32">
+        <v>42849</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="23">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
@@ -3082,7 +3092,7 @@
       <c r="B37" s="25"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Mécanisme de complétion des examens + Idée de récompense
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -237,12 +237,15 @@
   </si>
   <si>
     <t>Ajout des examens + début du layout pour les faire.</t>
+  </si>
+  <si>
+    <t>Mécanisme de completion des examens commencer + idée de récompense.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -380,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,7 +462,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +505,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -565,7 +573,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -631,7 +639,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -705,7 +713,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -773,7 +781,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -839,7 +847,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -913,7 +921,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -981,7 +989,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1047,7 +1055,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1121,7 +1129,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1189,7 +1197,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,7 +1263,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1329,7 +1337,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1397,7 +1405,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1463,7 +1471,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1593,6 +1601,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1628,6 +1653,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1810,45 +1852,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1859,7 +1901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1870,7 +1912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1881,7 +1923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1892,7 +1934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1903,7 +1945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1914,7 +1956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>9</v>
       </c>
@@ -1924,19 +1966,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1947,7 +1989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1958,7 +2000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1969,7 +2011,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1980,7 +2022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -1991,7 +2033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -2002,7 +2044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -2013,21 +2055,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>9</v>
       </c>
@@ -2037,7 +2079,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -2062,19 +2104,19 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2082,7 +2124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2090,7 +2132,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2098,13 +2140,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2115,7 +2157,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2126,7 +2168,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2137,7 +2179,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2148,7 +2190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2159,7 +2201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2170,7 +2212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>42771</v>
       </c>
@@ -2181,7 +2223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>42772</v>
       </c>
@@ -2192,7 +2234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>42773</v>
       </c>
@@ -2203,7 +2245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>42779</v>
       </c>
@@ -2214,72 +2256,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>9</v>
       </c>
@@ -2289,13 +2331,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2303,10 +2345,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2314,19 +2356,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="27"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="28"/>
     </row>
   </sheetData>
@@ -2348,19 +2390,19 @@
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2368,7 +2410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2376,7 +2418,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2384,13 +2426,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2401,7 +2443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42797</v>
       </c>
@@ -2412,7 +2454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>42797</v>
       </c>
@@ -2423,7 +2465,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>42797</v>
       </c>
@@ -2434,7 +2476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>42798</v>
       </c>
@@ -2445,7 +2487,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>42808</v>
       </c>
@@ -2456,7 +2498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>42814</v>
       </c>
@@ -2467,92 +2509,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
@@ -2562,13 +2604,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2576,10 +2618,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
@@ -2587,19 +2629,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="27"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="27"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="27"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="27"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="28"/>
     </row>
   </sheetData>
@@ -2621,19 +2663,19 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2641,7 +2683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2649,7 +2691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2657,13 +2699,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2674,7 +2716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42814</v>
       </c>
@@ -2685,7 +2727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42815</v>
       </c>
@@ -2696,7 +2738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42821</v>
       </c>
@@ -2707,7 +2749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42822</v>
       </c>
@@ -2718,7 +2760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>42797</v>
       </c>
@@ -2729,7 +2771,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>42830</v>
       </c>
@@ -2740,7 +2782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>42833</v>
       </c>
@@ -2751,7 +2793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>42834</v>
       </c>
@@ -2762,7 +2804,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>42834</v>
       </c>
@@ -2773,70 +2815,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>9</v>
       </c>
@@ -2846,13 +2888,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2860,10 +2902,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2871,19 +2913,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="30"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="31"/>
     </row>
   </sheetData>
@@ -2901,23 +2943,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2925,7 +2967,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2933,7 +2975,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2941,13 +2983,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2958,7 +3000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42836</v>
       </c>
@@ -2969,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="32">
         <v>42849</v>
       </c>
@@ -2980,155 +3022,161 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="23"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <v>42849</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
       <c r="B17" s="4"/>
       <c r="C17" s="23"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
       <c r="B18" s="4"/>
       <c r="C18" s="23"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
       <c r="B19" s="4"/>
       <c r="C19" s="23"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
       <c r="B20" s="4"/>
       <c r="C20" s="23"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
       <c r="B21" s="4"/>
       <c r="C21" s="23"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="33"/>
       <c r="B22" s="4"/>
       <c r="C22" s="23"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="33"/>
       <c r="B23" s="4"/>
       <c r="C23" s="23"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
       <c r="B24" s="4"/>
       <c r="C24" s="23"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="33"/>
       <c r="B25" s="4"/>
       <c r="C25" s="23"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
       <c r="B26" s="4"/>
       <c r="C26" s="23"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="33"/>
       <c r="B27" s="4"/>
       <c r="C27" s="23"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="33"/>
       <c r="B28" s="4"/>
       <c r="C28" s="23"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
       <c r="B29" s="4"/>
       <c r="C29" s="23"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
       <c r="B30" s="4"/>
       <c r="C30" s="23"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
       <c r="B31" s="4"/>
       <c r="C31" s="23"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
       <c r="B32" s="4"/>
       <c r="C32" s="23"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
       <c r="B33" s="4"/>
       <c r="C33" s="23"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
       <c r="B34" s="4"/>
       <c r="C34" s="23"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="33"/>
       <c r="B35" s="4"/>
       <c r="C35" s="23"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="33"/>
       <c r="B36" s="4"/>
       <c r="C36" s="23"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="29"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="30"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="30"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Condition de fin des examens + Puissance du click selon la connaissance
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -240,12 +240,15 @@
   </si>
   <si>
     <t>Mécanisme de completion des examens commencer + idée de récompense.</t>
+  </si>
+  <si>
+    <t>Condition de fin des examens + puissance du click selon la connaissance.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -438,6 +441,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -460,12 +469,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -505,7 +508,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -573,7 +576,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -639,7 +642,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -713,7 +716,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -781,7 +784,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -847,7 +850,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -921,7 +924,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -989,7 +992,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1055,7 +1058,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1129,7 +1132,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1197,7 +1200,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1263,7 +1266,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1337,7 +1340,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1405,7 +1408,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1471,7 +1474,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1601,23 +1604,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1653,23 +1639,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1852,45 +1821,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1901,7 +1870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1912,7 +1881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1923,7 +1892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1934,7 +1903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1945,7 +1914,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1956,29 +1925,29 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="24" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="25"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1989,7 +1958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -2000,7 +1969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -2011,7 +1980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -2022,7 +1991,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -2033,7 +2002,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -2044,7 +2013,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -2055,31 +2024,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="25"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -2104,19 +2073,19 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2124,7 +2093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2132,7 +2101,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2140,13 +2109,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2157,7 +2126,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2168,7 +2137,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2179,7 +2148,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2190,7 +2159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2201,7 +2170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2212,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>42771</v>
       </c>
@@ -2223,7 +2192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>42772</v>
       </c>
@@ -2234,7 +2203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>42773</v>
       </c>
@@ -2245,7 +2214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>42779</v>
       </c>
@@ -2256,88 +2225,88 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="16">
         <f>SUM(C14:C35)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2345,31 +2314,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="27"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="27"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="27"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="27"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="28"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="29"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="29"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="29"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="29"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2390,19 +2359,19 @@
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2410,7 +2379,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2418,7 +2387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2426,13 +2395,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2443,7 +2412,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42797</v>
       </c>
@@ -2454,7 +2423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <v>42797</v>
       </c>
@@ -2465,7 +2434,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>42797</v>
       </c>
@@ -2476,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>42798</v>
       </c>
@@ -2487,7 +2456,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>42808</v>
       </c>
@@ -2498,7 +2467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>42814</v>
       </c>
@@ -2509,108 +2478,108 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="22"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="25"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="10">
         <f>SUM(C14:C36)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2618,31 +2587,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="26" t="s">
+      <c r="B42" s="28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="27"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="27"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="27"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="27"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="28"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="29"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="29"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="29"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="29"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2663,19 +2632,19 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2683,7 +2652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2691,7 +2660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2699,13 +2668,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2716,7 +2685,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42814</v>
       </c>
@@ -2727,7 +2696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42815</v>
       </c>
@@ -2738,7 +2707,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42821</v>
       </c>
@@ -2749,7 +2718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42822</v>
       </c>
@@ -2760,7 +2729,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42797</v>
       </c>
@@ -2771,7 +2740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>42830</v>
       </c>
@@ -2782,7 +2751,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>42833</v>
       </c>
@@ -2793,7 +2762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>42834</v>
       </c>
@@ -2804,7 +2773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="20">
         <v>42834</v>
       </c>
@@ -2815,86 +2784,86 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="25"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="10">
         <f>SUM(C14:C35)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2902,31 +2871,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="30"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="30"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="31"/>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="32"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="32"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="32"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="32"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2944,22 +2913,22 @@
   <dimension ref="A6:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2967,7 +2936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2975,7 +2944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2983,13 +2952,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -3000,7 +2969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42836</v>
       </c>
@@ -3011,8 +2980,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="32">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="24">
         <v>42849</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -3022,8 +2991,8 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="24">
         <v>42849</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -3033,151 +3002,157 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="23"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="24">
+        <v>42850</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="25"/>
       <c r="B18" s="4"/>
       <c r="C18" s="23"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="25"/>
       <c r="B19" s="4"/>
       <c r="C19" s="23"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="25"/>
       <c r="B20" s="4"/>
       <c r="C20" s="23"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="25"/>
       <c r="B21" s="4"/>
       <c r="C21" s="23"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="25"/>
       <c r="B22" s="4"/>
       <c r="C22" s="23"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="33"/>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
       <c r="B23" s="4"/>
       <c r="C23" s="23"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
       <c r="B24" s="4"/>
       <c r="C24" s="23"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="25"/>
       <c r="B25" s="4"/>
       <c r="C25" s="23"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
       <c r="B26" s="4"/>
       <c r="C26" s="23"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="25"/>
       <c r="B27" s="4"/>
       <c r="C27" s="23"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="25"/>
       <c r="B28" s="4"/>
       <c r="C28" s="23"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="25"/>
       <c r="B29" s="4"/>
       <c r="C29" s="23"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
       <c r="B30" s="4"/>
       <c r="C30" s="23"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="25"/>
       <c r="B31" s="4"/>
       <c r="C31" s="23"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="25"/>
       <c r="B32" s="4"/>
       <c r="C32" s="23"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="25"/>
       <c r="B33" s="4"/>
       <c r="C33" s="23"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="25"/>
       <c r="B34" s="4"/>
       <c r="C34" s="23"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="25"/>
       <c r="B35" s="4"/>
       <c r="C35" s="23"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="25"/>
       <c r="B36" s="4"/>
       <c r="C36" s="23"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="25"/>
+      <c r="B37" s="27"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="29"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="30"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="30"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="30"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="31"/>
+      <c r="B42" s="31"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="32"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="32"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="32"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="32"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Création d'un MessageBox pour afficher les messages + implémentation de celui-ci.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Condition de fin des examens + puissance du click selon la connaissance.</t>
+  </si>
+  <si>
+    <t>Création d'un MessageBox pour afficher les messages + implémentation de celui-ci.</t>
   </si>
 </sst>
 </file>
@@ -2912,8 +2915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3014,9 +3017,15 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="23"/>
+      <c r="A18" s="24">
+        <v>42850</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" s="23">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="25"/>
@@ -3115,7 +3124,7 @@
       <c r="B37" s="27"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>6</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Les examens se terminent selon un chrono + Implémentation d'une animation pour les progress bars.
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -246,12 +246,15 @@
   </si>
   <si>
     <t>Création d'un MessageBox pour afficher les messages + implémentation de celui-ci.</t>
+  </si>
+  <si>
+    <t>Les examens se terminent selon un chrono + Implémentation d'une animation pour les progress bars.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -511,7 +514,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -579,7 +582,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -645,7 +648,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -719,7 +722,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -787,7 +790,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -853,7 +856,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -927,7 +930,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -995,7 +998,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,7 +1064,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1135,7 +1138,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1203,7 +1206,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1269,7 +1272,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1343,7 +1346,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1411,7 +1414,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1477,7 +1480,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1607,6 +1610,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1642,6 +1662,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1824,45 +1861,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1873,7 +1910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1884,7 +1921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1895,7 +1932,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1906,7 +1943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1917,7 +1954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1928,7 +1965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="26" t="s">
         <v>9</v>
       </c>
@@ -1938,19 +1975,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1961,7 +1998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1972,7 +2009,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1983,7 +2020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1994,7 +2031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -2005,7 +2042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -2016,7 +2053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -2027,21 +2064,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="26" t="s">
         <v>9</v>
       </c>
@@ -2051,7 +2088,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -2076,19 +2113,19 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2096,7 +2133,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2104,7 +2141,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2112,13 +2149,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2129,7 +2166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2140,7 +2177,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2151,7 +2188,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2162,7 +2199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2173,7 +2210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2184,7 +2221,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>42771</v>
       </c>
@@ -2195,7 +2232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>42772</v>
       </c>
@@ -2206,7 +2243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>42773</v>
       </c>
@@ -2217,7 +2254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>42779</v>
       </c>
@@ -2228,72 +2265,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
@@ -2303,13 +2340,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2317,10 +2354,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2328,19 +2365,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="29"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="29"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="29"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="29"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="30"/>
     </row>
   </sheetData>
@@ -2362,19 +2399,19 @@
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2382,7 +2419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2390,7 +2427,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2398,13 +2435,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2415,7 +2452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42797</v>
       </c>
@@ -2426,7 +2463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>42797</v>
       </c>
@@ -2437,7 +2474,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>42797</v>
       </c>
@@ -2448,7 +2485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>42798</v>
       </c>
@@ -2459,7 +2496,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>42808</v>
       </c>
@@ -2470,7 +2507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>42814</v>
       </c>
@@ -2481,92 +2518,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="22"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
         <v>9</v>
       </c>
@@ -2576,13 +2613,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2590,10 +2627,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
@@ -2601,19 +2638,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="29"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="29"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="29"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="29"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="30"/>
     </row>
   </sheetData>
@@ -2635,19 +2672,19 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2655,7 +2692,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2663,7 +2700,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2671,13 +2708,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2688,7 +2725,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42814</v>
       </c>
@@ -2699,7 +2736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>42815</v>
       </c>
@@ -2710,7 +2747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>42821</v>
       </c>
@@ -2721,7 +2758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>42822</v>
       </c>
@@ -2732,7 +2769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>42797</v>
       </c>
@@ -2743,7 +2780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>42830</v>
       </c>
@@ -2754,7 +2791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>42833</v>
       </c>
@@ -2765,7 +2802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>42834</v>
       </c>
@@ -2776,7 +2813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>42834</v>
       </c>
@@ -2787,70 +2824,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
@@ -2860,13 +2897,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2874,10 +2911,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2885,19 +2922,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="32"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="33"/>
     </row>
   </sheetData>
@@ -2913,25 +2950,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:C47"/>
+  <dimension ref="A6:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2939,7 +2976,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2947,7 +2984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2955,13 +2992,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2972,7 +3009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42836</v>
       </c>
@@ -2983,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>42849</v>
       </c>
@@ -2994,7 +3031,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
         <v>42849</v>
       </c>
@@ -3005,7 +3042,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>42850</v>
       </c>
@@ -3016,7 +3053,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>42850</v>
       </c>
@@ -3027,146 +3064,147 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="23"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>42855</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="4"/>
       <c r="C20" s="23"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="4"/>
       <c r="C21" s="23"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="4"/>
       <c r="C22" s="23"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="4"/>
       <c r="C23" s="23"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="4"/>
       <c r="C24" s="23"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="4"/>
       <c r="C25" s="23"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="4"/>
       <c r="C26" s="23"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="4"/>
       <c r="C27" s="23"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
       <c r="B28" s="4"/>
       <c r="C28" s="23"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="4"/>
       <c r="C29" s="23"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
       <c r="B30" s="4"/>
       <c r="C30" s="23"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
       <c r="B31" s="4"/>
       <c r="C31" s="23"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="4"/>
       <c r="C32" s="23"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="4"/>
       <c r="C33" s="23"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="4"/>
       <c r="C34" s="23"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
       <c r="B35" s="4"/>
       <c r="C35" s="23"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="23"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="16">
-        <f>SUM(C14:C36)</f>
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="B36" s="27"/>
+      <c r="C36" s="16">
+        <f>SUM(C14:C35)</f>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="17"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="B39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="31"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="31"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="32"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="32"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="32"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="32"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" s="32"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B47" s="33"/>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="B41:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Léger nettoyage de code + condition de fin du jeu (Réussite ou échec)
</commit_message>
<xml_diff>
--- a/Itérations.xlsx
+++ b/Itérations.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8025" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8028" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="78">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -249,12 +249,15 @@
   </si>
   <si>
     <t>Les examens se terminent selon un chrono + Implémentation d'une animation pour les progress bars.</t>
+  </si>
+  <si>
+    <t>Léger nettoyage de code + condition de fin du jeu (Réussite ou échec)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -514,7 +517,7 @@
         <xdr:cNvPr id="1026" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -582,7 +585,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -648,7 +651,7 @@
         <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -722,7 +725,7 @@
         <xdr:cNvPr id="5" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -790,7 +793,7 @@
         <xdr:cNvPr id="6" name="ZoneTexte 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -856,7 +859,7 @@
         <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -930,7 +933,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -998,7 +1001,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1064,7 +1067,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1138,7 +1141,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1206,7 +1209,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1272,7 +1275,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1346,7 +1349,7 @@
         <xdr:cNvPr id="2" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1414,7 +1417,7 @@
         <xdr:cNvPr id="3" name="ZoneTexte 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1480,7 +1483,7 @@
         <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1610,23 +1613,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1662,23 +1648,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1861,45 +1830,45 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.44140625" customWidth="1"/>
+    <col min="2" max="2" width="64.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1910,7 +1879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1921,7 +1890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1932,7 +1901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1943,7 +1912,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1954,7 +1923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1965,7 +1934,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>9</v>
       </c>
@@ -1975,19 +1944,19 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1998,7 +1967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -2009,7 +1978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -2020,7 +1989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -2031,7 +2000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>4</v>
       </c>
@@ -2042,7 +2011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>5</v>
       </c>
@@ -2053,7 +2022,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>6</v>
       </c>
@@ -2064,21 +2033,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
         <v>9</v>
       </c>
@@ -2088,7 +2057,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -2113,19 +2082,19 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2133,7 +2102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2141,7 +2110,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2149,13 +2118,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2166,7 +2135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -2177,7 +2146,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42765</v>
       </c>
@@ -2188,7 +2157,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42765</v>
       </c>
@@ -2199,7 +2168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42766</v>
       </c>
@@ -2210,7 +2179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42766</v>
       </c>
@@ -2221,7 +2190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>42771</v>
       </c>
@@ -2232,7 +2201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>42772</v>
       </c>
@@ -2243,7 +2212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>42773</v>
       </c>
@@ -2254,7 +2223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>42779</v>
       </c>
@@ -2265,72 +2234,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
@@ -2340,13 +2309,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2354,10 +2323,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2365,19 +2334,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="29"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="29"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="29"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="29"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="30"/>
     </row>
   </sheetData>
@@ -2399,19 +2368,19 @@
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2419,7 +2388,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2427,7 +2396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2435,13 +2404,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2452,7 +2421,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42797</v>
       </c>
@@ -2463,7 +2432,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="20">
         <v>42797</v>
       </c>
@@ -2474,7 +2443,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="20">
         <v>42797</v>
       </c>
@@ -2485,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>42798</v>
       </c>
@@ -2496,7 +2465,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="20">
         <v>42808</v>
       </c>
@@ -2507,7 +2476,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>42814</v>
       </c>
@@ -2518,92 +2487,92 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="22"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="4"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="26" t="s">
         <v>9</v>
       </c>
@@ -2613,13 +2582,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2627,10 +2596,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
@@ -2638,19 +2607,19 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="29"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="29"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="29"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="29"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="30"/>
     </row>
   </sheetData>
@@ -2672,19 +2641,19 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2692,7 +2661,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2700,7 +2669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2708,13 +2677,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2725,7 +2694,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42814</v>
       </c>
@@ -2736,7 +2705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>42815</v>
       </c>
@@ -2747,7 +2716,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>42821</v>
       </c>
@@ -2758,7 +2727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>42822</v>
       </c>
@@ -2769,7 +2738,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>42797</v>
       </c>
@@ -2780,7 +2749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>42830</v>
       </c>
@@ -2791,7 +2760,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>42833</v>
       </c>
@@ -2802,7 +2771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>42834</v>
       </c>
@@ -2813,7 +2782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="20">
         <v>42834</v>
       </c>
@@ -2824,70 +2793,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19"/>
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="19"/>
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19"/>
       <c r="B26" s="4"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="19"/>
       <c r="B27" s="4"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19"/>
       <c r="B28" s="4"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="19"/>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19"/>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="19"/>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19"/>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="19"/>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="19"/>
       <c r="B34" s="4"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="19"/>
       <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
@@ -2897,13 +2866,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
@@ -2911,10 +2880,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
@@ -2922,19 +2891,19 @@
         <v>69</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="32"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="32"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="32"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="32"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="33"/>
     </row>
   </sheetData>
@@ -2953,22 +2922,22 @@
   <dimension ref="A6:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="70.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2976,7 +2945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2984,7 +2953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2992,13 +2961,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -3009,7 +2978,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>42836</v>
       </c>
@@ -3020,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="24">
         <v>42849</v>
       </c>
@@ -3031,7 +3000,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="24">
         <v>42849</v>
       </c>
@@ -3042,7 +3011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="24">
         <v>42850</v>
       </c>
@@ -3053,7 +3022,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="24">
         <v>42850</v>
       </c>
@@ -3064,7 +3033,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="20">
         <v>42855</v>
       </c>
@@ -3075,130 +3044,136 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="23"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="24">
+        <v>42856</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="25"/>
       <c r="B21" s="4"/>
       <c r="C21" s="23"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="25"/>
       <c r="B22" s="4"/>
       <c r="C22" s="23"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="25"/>
       <c r="B23" s="4"/>
       <c r="C23" s="23"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="25"/>
       <c r="B24" s="4"/>
       <c r="C24" s="23"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
       <c r="B25" s="4"/>
       <c r="C25" s="23"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="25"/>
       <c r="B26" s="4"/>
       <c r="C26" s="23"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="25"/>
       <c r="B27" s="4"/>
       <c r="C27" s="23"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="25"/>
       <c r="B28" s="4"/>
       <c r="C28" s="23"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="25"/>
       <c r="B29" s="4"/>
       <c r="C29" s="23"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="25"/>
       <c r="B30" s="4"/>
       <c r="C30" s="23"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="25"/>
       <c r="B31" s="4"/>
       <c r="C31" s="23"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="25"/>
       <c r="B32" s="4"/>
       <c r="C32" s="23"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="25"/>
       <c r="B33" s="4"/>
       <c r="C33" s="23"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="25"/>
       <c r="B34" s="4"/>
       <c r="C34" s="23"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="25"/>
       <c r="B35" s="4"/>
       <c r="C35" s="23"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="26" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="27"/>
       <c r="C36" s="16">
         <f>SUM(C14:C35)</f>
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="4"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B41" s="31"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="32"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="32"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="32"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="32"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="33"/>
     </row>
   </sheetData>

</xml_diff>